<commit_message>
every 1 min sends email
</commit_message>
<xml_diff>
--- a/ExcelReport/Reports.xlsx
+++ b/ExcelReport/Reports.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Daily Download Report</t>
   </si>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t>DownloadCount</t>
-  </si>
-  <si>
-    <t>31.7.2023 0:00:00</t>
-  </si>
-  <si>
-    <t>C# 10 in a Nutshell The Definitive Reference Joseph Albahari</t>
   </si>
 </sst>
 </file>
@@ -95,14 +89,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.554903030395508" customWidth="1" style="1"/>
-    <col min="2" max="2" width="53.43231201171875" customWidth="1"/>
+    <col min="1" max="1" width="13.7987642288208" customWidth="1" style="1"/>
+    <col min="2" max="2" width="14.022814750671387" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -122,17 +116,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
background task report working(makeing report and sending it after 20 sec)
</commit_message>
<xml_diff>
--- a/ExcelReport/Reports.xlsx
+++ b/ExcelReport/Reports.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Daily Download Report</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>DownloadCount</t>
+  </si>
+  <si>
+    <t>1.8.2023 0:00:00</t>
+  </si>
+  <si>
+    <t>C# 10 in a Nutshell The Definitive Reference Joseph Albahari</t>
   </si>
 </sst>
 </file>
@@ -89,14 +95,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7987642288208" customWidth="1" style="1"/>
-    <col min="2" max="2" width="14.022814750671387" customWidth="1"/>
+    <col min="1" max="1" width="15.461244583129883" customWidth="1" style="1"/>
+    <col min="2" max="2" width="53.43231201171875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -116,6 +122,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
report generator fully working
</commit_message>
<xml_diff>
--- a/ExcelReport/Reports.xlsx
+++ b/ExcelReport/Reports.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Daily Download Report</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>DownloadCount</t>
+  </si>
+  <si>
+    <t>1.8.2023 0:00:00</t>
+  </si>
+  <si>
+    <t>C# 10 in a Nutshell The Definitive Reference Joseph Albahari</t>
   </si>
 </sst>
 </file>
@@ -89,14 +95,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7987642288208" customWidth="1" style="1"/>
-    <col min="2" max="2" width="14.022814750671387" customWidth="1"/>
+    <col min="1" max="1" width="15.461244583129883" customWidth="1" style="1"/>
+    <col min="2" max="2" width="53.43231201171875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -116,6 +122,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:C1"/>

</xml_diff>